<commit_message>
added sheet for analog transfer function
</commit_message>
<xml_diff>
--- a/instrument_info.xlsx
+++ b/instrument_info.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HERAMB\Desktop\pandas\timesequence program copy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HERAMB\cold atom exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2058F3CA-BC5E-4279-A2EB-020E46136EAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE0620F-9455-4B6B-A24B-BAD6CCB107FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instrument_info" sheetId="1" r:id="rId1"/>
+    <sheet name="instrument_calib" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -71,6 +72,15 @@
   </si>
   <si>
     <t>image beam</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>Instrument name</t>
+  </si>
+  <si>
+    <t>[0,1]</t>
   </si>
 </sst>
 </file>
@@ -935,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,4 +1149,39 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF22C71-6FD8-4642-B658-07CB75A63290}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
instrument transfer function information
</commit_message>
<xml_diff>
--- a/instrument_info.xlsx
+++ b/instrument_info.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HERAMB\cold atom exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE0620F-9455-4B6B-A24B-BAD6CCB107FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57822A94-8EE7-4BBC-8D0A-9169C8C07098}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instrument_info" sheetId="1" r:id="rId1"/>
-    <sheet name="instrument_calib" sheetId="2" r:id="rId2"/>
+    <sheet name="instrument_transfer" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -1156,7 +1156,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modified Instrument_info according for requirement of analog transfer function
</commit_message>
<xml_diff>
--- a/instrument_info.xlsx
+++ b/instrument_info.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IITG-PHY\Desktop\Computer Control\cold atom exp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\Computer Control\programs\python programs\cold-atom-exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAA5CD3-C6FA-4518-A85B-0EDC29523068}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E85489-7C35-4870-BD09-A8579190311F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instrument_info" sheetId="1" r:id="rId1"/>
+    <sheet name="instrument_function" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="137">
   <si>
     <t>name</t>
   </si>
@@ -401,6 +402,36 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>coeffs</t>
+  </si>
+  <si>
+    <t>poly</t>
+  </si>
+  <si>
+    <t>[1,1]</t>
+  </si>
+  <si>
+    <t>[0,1]</t>
+  </si>
+  <si>
+    <t>[2,1]</t>
+  </si>
+  <si>
+    <t>[-1,1]</t>
+  </si>
+  <si>
+    <t>[1,2]</t>
+  </si>
+  <si>
+    <t>[0.5,0.5]</t>
+  </si>
+  <si>
+    <t>[0,0.5]</t>
   </si>
 </sst>
 </file>
@@ -1243,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F121"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3677,4 +3708,470 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A89B4C-2FE4-476C-989E-0471C5FB2646}">
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modified instru for time sequnce
</commit_message>
<xml_diff>
--- a/instrument_info.xlsx
+++ b/instrument_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\Computer Control\programs\python programs\cold-atom-exp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IITG-PHY\Desktop\Computer Control\cold atom exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E85489-7C35-4870-BD09-A8579190311F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2839B2-37DF-4B5C-A40A-52CE6D5F93D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instrument_info" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="142">
   <si>
     <t>name</t>
   </si>
@@ -432,6 +432,21 @@
   </si>
   <si>
     <t>[0,0.5]</t>
+  </si>
+  <si>
+    <t>img_s</t>
+  </si>
+  <si>
+    <t>Do not connect</t>
+  </si>
+  <si>
+    <t>ccd</t>
+  </si>
+  <si>
+    <t>mot_s</t>
+  </si>
+  <si>
+    <t>mag_s</t>
   </si>
 </sst>
 </file>
@@ -915,8 +930,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1274,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,7 +2598,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -2601,8 +2617,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>71</v>
+      <c r="A67" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -2622,7 +2638,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -2642,7 +2658,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>140</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -2662,7 +2678,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -3714,7 +3730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A89B4C-2FE4-476C-989E-0471C5FB2646}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8:C41"/>
     </sheetView>
   </sheetViews>

</xml_diff>